<commit_message>
Curso Docker 2022 - Iconos
</commit_message>
<xml_diff>
--- a/00soportes/Portafolio/Carrera propuesta para Desarrollador web/Ruta Desarrollo Web.xlsx
+++ b/00soportes/Portafolio/Carrera propuesta para Desarrollador web/Ruta Desarrollo Web.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\cvpetrix2022\00soportes\Portafolio\Carrera propuesta para Desarrollador web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF7B44E-1120-455E-B0D2-12C532C9A342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B76B59-7F75-4AD7-B173-5ABCF2D5E2C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -40,8 +40,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3426,9 +3424,6 @@
     <t>'php','mysql','javascript','facebook','google','fireabase'</t>
   </si>
   <si>
-    <t>'docker','laravel','mongodb','phyton','mysql'</t>
-  </si>
-  <si>
     <t>https://www.udemy.com/course/lenguaje-go</t>
   </si>
   <si>
@@ -4012,6 +4007,9 @@
   </si>
   <si>
     <t>https://github.com/petrix12/docker2022</t>
+  </si>
+  <si>
+    <t>'docker','laravel','mongo','python','mysql'</t>
   </si>
 </sst>
 </file>
@@ -6186,7 +6184,7 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -6201,7 +6199,7 @@
       </c>
       <c r="B1" s="13">
         <f ca="1">TODAY()</f>
-        <v>44922</v>
+        <v>44925</v>
       </c>
       <c r="E1" s="21">
         <f>SUMIF(courses!J:J,1,courses!K:K)/60</f>
@@ -6803,11 +6801,11 @@
   </sheetPr>
   <dimension ref="A1:AZ244"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="P210" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="P209" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A214" sqref="A214"/>
+      <selection pane="bottomRight" activeCell="V214" sqref="V214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12625,7 +12623,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="C36" t="s">
         <v>260</v>
@@ -12634,7 +12632,7 @@
         <v>317</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="F36" t="s">
         <v>8</v>
@@ -12656,10 +12654,10 @@
         <v>93</v>
       </c>
       <c r="O36" t="s">
+        <v>1278</v>
+      </c>
+      <c r="P36" t="s">
         <v>1279</v>
-      </c>
-      <c r="P36" t="s">
-        <v>1280</v>
       </c>
       <c r="R36" t="s">
         <v>433</v>
@@ -21555,7 +21553,7 @@
         <v>265</v>
       </c>
       <c r="P90" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="R90" t="s">
         <v>433</v>
@@ -23708,7 +23706,7 @@
         <v>373</v>
       </c>
       <c r="F103" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="G103" s="3">
         <v>0</v>
@@ -24224,7 +24222,7 @@
         <v>388</v>
       </c>
       <c r="F106" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="G106" s="3">
         <v>0</v>
@@ -24394,7 +24392,7 @@
         <v>392</v>
       </c>
       <c r="F107" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="G107" s="3">
         <v>0</v>
@@ -25381,7 +25379,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C113" t="s">
         <v>333</v>
@@ -25915,7 +25913,7 @@
         <v>448</v>
       </c>
       <c r="F116" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="G116" s="3">
         <v>0</v>
@@ -28678,7 +28676,7 @@
         <v>147</v>
       </c>
       <c r="O132" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="P132" t="s">
         <v>1016</v>
@@ -28847,7 +28845,7 @@
         <v>147</v>
       </c>
       <c r="O133" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="P133" t="s">
         <v>1017</v>
@@ -29016,7 +29014,7 @@
         <v>147</v>
       </c>
       <c r="O134" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="P134" t="s">
         <v>1018</v>
@@ -29185,7 +29183,7 @@
         <v>147</v>
       </c>
       <c r="O135" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="P135" t="s">
         <v>1019</v>
@@ -29354,7 +29352,7 @@
         <v>147</v>
       </c>
       <c r="O136" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="P136" t="s">
         <v>1020</v>
@@ -29694,7 +29692,7 @@
         <v>147</v>
       </c>
       <c r="O138" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="P138" t="s">
         <v>1022</v>
@@ -30707,7 +30705,7 @@
         <v>147</v>
       </c>
       <c r="O144" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="P144" t="s">
         <v>1027</v>
@@ -30876,7 +30874,7 @@
         <v>147</v>
       </c>
       <c r="O145" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="P145" t="s">
         <v>1028</v>
@@ -32765,7 +32763,7 @@
         <v>590</v>
       </c>
       <c r="N156" s="2" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="O156" t="s">
         <v>48</v>
@@ -32792,7 +32790,7 @@
         <v>15</v>
       </c>
       <c r="X156" s="2" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="AA156" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -33945,7 +33943,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="19" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="C163" t="s">
         <v>435</v>
@@ -33978,7 +33976,7 @@
         <v>44082</v>
       </c>
       <c r="N163" s="2" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="O163" t="s">
         <v>627</v>
@@ -34147,7 +34145,7 @@
         <v>44082</v>
       </c>
       <c r="N164" s="2" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="O164" t="s">
         <v>631</v>
@@ -34836,7 +34834,7 @@
         <v>44068</v>
       </c>
       <c r="N168" s="2" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="O168" t="s">
         <v>495</v>
@@ -35182,7 +35180,7 @@
         <v>44076</v>
       </c>
       <c r="N170" s="2" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="O170" t="s">
         <v>666</v>
@@ -35525,7 +35523,7 @@
         <v>44059</v>
       </c>
       <c r="N172" s="2" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="O172" t="s">
         <v>675</v>
@@ -35695,7 +35693,7 @@
         <v>44056</v>
       </c>
       <c r="N173" s="2" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="O173" t="s">
         <v>679</v>
@@ -36038,10 +36036,10 @@
         <v>44649</v>
       </c>
       <c r="M175" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="N175" s="2" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="O175" t="s">
         <v>1058</v>
@@ -36542,13 +36540,13 @@
         <v>44846</v>
       </c>
       <c r="M178" t="s">
+        <v>1288</v>
+      </c>
+      <c r="N178" s="2" t="s">
         <v>1289</v>
       </c>
-      <c r="N178" s="2" t="s">
+      <c r="O178" t="s">
         <v>1290</v>
-      </c>
-      <c r="O178" t="s">
-        <v>1291</v>
       </c>
       <c r="P178" t="s">
         <v>691</v>
@@ -36566,13 +36564,13 @@
         <v>783</v>
       </c>
       <c r="V178" s="19" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="W178" s="19" t="s">
         <v>15</v>
       </c>
       <c r="X178" s="2" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="AA178" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -40013,7 +40011,7 @@
         <v>40066</v>
       </c>
       <c r="O199" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="P199" t="s">
         <v>760</v>
@@ -41986,13 +41984,13 @@
         <v>44660</v>
       </c>
       <c r="M211" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="N211" s="2" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="O211" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="P211" t="s">
         <v>1055</v>
@@ -42016,7 +42014,7 @@
         <v>14</v>
       </c>
       <c r="X211" s="2" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="AA211" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -42326,10 +42324,10 @@
         <v>44873</v>
       </c>
       <c r="M213" t="s">
+        <v>1300</v>
+      </c>
+      <c r="N213" s="2" t="s">
         <v>1301</v>
-      </c>
-      <c r="N213" s="2" t="s">
-        <v>1302</v>
       </c>
       <c r="O213" t="s">
         <v>30</v>
@@ -42350,13 +42348,13 @@
         <v>783</v>
       </c>
       <c r="V213" s="19" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="W213" t="s">
         <v>14</v>
       </c>
       <c r="X213" s="2" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="AA213" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -42502,10 +42500,10 @@
         <v>44922</v>
       </c>
       <c r="M214" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="N214" s="2" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="O214" t="s">
         <v>431</v>
@@ -42526,13 +42524,13 @@
         <v>783</v>
       </c>
       <c r="V214" s="19" t="s">
-        <v>1125</v>
+        <v>1320</v>
       </c>
       <c r="W214" t="s">
         <v>14</v>
       </c>
       <c r="X214" s="2" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="AA214" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -42620,7 +42618,7 @@
       </c>
       <c r="AV214" t="str">
         <f>AV$1&amp;": [ "&amp;Tabla5[[#This Row],[logo_technologies]]&amp;" ], "</f>
-        <v xml:space="preserve">logo_technologies: [ 'docker','laravel','mongodb','phyton','mysql' ], </v>
+        <v xml:space="preserve">logo_technologies: [ 'docker','laravel','mongo','python','mysql' ], </v>
       </c>
       <c r="AW214" t="str">
         <f>AW$1&amp;": "&amp;Tabla5[[#This Row],[mostrar]]&amp;", "</f>
@@ -42636,7 +42634,7 @@
       </c>
       <c r="AZ214" t="str">
         <f t="shared" ref="AZ214" si="4">"{ "&amp;AA214&amp;AB214&amp;AC214&amp;AD214&amp;AE214&amp;AF214&amp;AG214&amp;AH214&amp;AI214&amp;AJ214&amp;AK214&amp;AL214&amp;AM214&amp;AN214&amp;AO214&amp;AP214&amp;AQ214&amp;AR214&amp;AS214&amp;AT214&amp;AU214&amp;AV214&amp;AW214&amp;AX214&amp;AY214&amp;" },"</f>
-        <v>{ id: 213, name: 'Curso práctico de Docker y Microservicios (apto para todos)', category: 'Herramientas', technology: 'Docker', url: 'https://www.udemy.com/course/curso-practico-de-docker-y-microservicios-desde-cero', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 0, minutos: 535, culminado: '2022-12-27', certificado: 'UC-d479ccde-befd-4a7d-9632-5b1debb609e0', url_certificado: 'https://udemy-certificate.s3.amazonaws.com/pdf/UC-d479ccde-befd-4a7d-9632-5b1debb609e0.pdf', instructor: 'Juan Ramos', description: 'Aprende por qué es importante, cómo funciona, y cómo empezar usar Docker en tus proyectos!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'docker','laravel','mongodb','phyton','mysql' ], mostrar: true, repositorio: 'https://github.com/petrix12/docker2022', nota: '' },</v>
+        <v>{ id: 213, name: 'Curso práctico de Docker y Microservicios (apto para todos)', category: 'Herramientas', technology: 'Docker', url: 'https://www.udemy.com/course/curso-practico-de-docker-y-microservicios-desde-cero', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 0, minutos: 535, culminado: '2022-12-27', certificado: 'UC-d479ccde-befd-4a7d-9632-5b1debb609e0', url_certificado: 'https://udemy-certificate.s3.amazonaws.com/pdf/UC-d479ccde-befd-4a7d-9632-5b1debb609e0.pdf', instructor: 'Juan Ramos', description: 'Aprende por qué es importante, cómo funciona, y cómo empezar usar Docker en tus proyectos!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'docker','laravel','mongo','python','mysql' ], mostrar: true, repositorio: 'https://github.com/petrix12/docker2022', nota: '' },</v>
       </c>
     </row>
     <row r="215" spans="1:52" x14ac:dyDescent="0.3">
@@ -42644,16 +42642,16 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="C215" t="s">
         <v>438</v>
       </c>
       <c r="D215" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="E215" s="2" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="F215" t="s">
         <v>8</v>
@@ -42675,10 +42673,10 @@
         <v>904</v>
       </c>
       <c r="O215" t="s">
+        <v>1161</v>
+      </c>
+      <c r="P215" t="s">
         <v>1162</v>
-      </c>
-      <c r="P215" t="s">
-        <v>1163</v>
       </c>
       <c r="R215" t="s">
         <v>433</v>
@@ -42693,7 +42691,7 @@
         <v>783</v>
       </c>
       <c r="V215" s="19" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="W215" t="s">
         <v>15</v>
@@ -42808,16 +42806,16 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="C216" t="s">
         <v>438</v>
       </c>
       <c r="D216" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="E216" s="2" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="F216" t="s">
         <v>8</v>
@@ -42839,10 +42837,10 @@
         <v>112</v>
       </c>
       <c r="O216" t="s">
+        <v>1176</v>
+      </c>
+      <c r="P216" t="s">
         <v>1177</v>
-      </c>
-      <c r="P216" t="s">
-        <v>1178</v>
       </c>
       <c r="R216" t="s">
         <v>433</v>
@@ -42857,7 +42855,7 @@
         <v>783</v>
       </c>
       <c r="V216" s="19" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="W216" t="s">
         <v>15</v>
@@ -42972,7 +42970,7 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="C217" t="s">
         <v>438</v>
@@ -42981,7 +42979,7 @@
         <v>440</v>
       </c>
       <c r="E217" s="2" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="F217" t="s">
         <v>8</v>
@@ -43006,7 +43004,7 @@
         <v>185</v>
       </c>
       <c r="P217" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="R217" t="s">
         <v>433</v>
@@ -43136,16 +43134,16 @@
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="C218" t="s">
         <v>438</v>
       </c>
       <c r="D218" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E218" s="2" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="F218" t="s">
         <v>8</v>
@@ -43167,10 +43165,10 @@
         <v>266</v>
       </c>
       <c r="O218" t="s">
+        <v>1189</v>
+      </c>
+      <c r="P218" t="s">
         <v>1190</v>
-      </c>
-      <c r="P218" t="s">
-        <v>1191</v>
       </c>
       <c r="R218" t="s">
         <v>433</v>
@@ -43185,7 +43183,7 @@
         <v>783</v>
       </c>
       <c r="V218" s="19" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="W218" t="s">
         <v>15</v>
@@ -43300,16 +43298,16 @@
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C219" t="s">
         <v>438</v>
       </c>
       <c r="D219" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E219" s="2" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="F219" t="s">
         <v>8</v>
@@ -43334,7 +43332,7 @@
         <v>160</v>
       </c>
       <c r="P219" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="R219" t="s">
         <v>433</v>
@@ -43349,7 +43347,7 @@
         <v>783</v>
       </c>
       <c r="V219" s="19" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="W219" t="s">
         <v>15</v>
@@ -43464,16 +43462,16 @@
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="C220" t="s">
         <v>333</v>
       </c>
       <c r="D220" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="E220" s="2" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="F220" t="s">
         <v>8</v>
@@ -43498,7 +43496,7 @@
         <v>185</v>
       </c>
       <c r="P220" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="R220" t="s">
         <v>433</v>
@@ -43513,7 +43511,7 @@
         <v>783</v>
       </c>
       <c r="V220" s="19" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="W220" t="s">
         <v>15</v>
@@ -43628,16 +43626,16 @@
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C221" t="s">
         <v>374</v>
       </c>
       <c r="D221" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="E221" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="F221" t="s">
         <v>8</v>
@@ -43659,10 +43657,10 @@
         <v>950</v>
       </c>
       <c r="O221" t="s">
+        <v>1171</v>
+      </c>
+      <c r="P221" t="s">
         <v>1172</v>
-      </c>
-      <c r="P221" t="s">
-        <v>1173</v>
       </c>
       <c r="R221" t="s">
         <v>433</v>
@@ -43677,7 +43675,7 @@
         <v>783</v>
       </c>
       <c r="V221" s="19" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="W221" t="s">
         <v>15</v>
@@ -43792,16 +43790,16 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="C222" t="s">
         <v>374</v>
       </c>
       <c r="D222" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="E222" s="2" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="F222" t="s">
         <v>8</v>
@@ -43823,10 +43821,10 @@
         <v>327</v>
       </c>
       <c r="O222" t="s">
+        <v>1206</v>
+      </c>
+      <c r="P222" t="s">
         <v>1207</v>
-      </c>
-      <c r="P222" t="s">
-        <v>1208</v>
       </c>
       <c r="R222" t="s">
         <v>433</v>
@@ -43841,7 +43839,7 @@
         <v>783</v>
       </c>
       <c r="V222" s="19" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="W222" t="s">
         <v>15</v>
@@ -43956,16 +43954,16 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="C223" t="s">
         <v>374</v>
       </c>
       <c r="D223" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E223" s="2" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="F223" t="s">
         <v>8</v>
@@ -43987,10 +43985,10 @@
         <v>412</v>
       </c>
       <c r="O223" t="s">
+        <v>1209</v>
+      </c>
+      <c r="P223" t="s">
         <v>1210</v>
-      </c>
-      <c r="P223" t="s">
-        <v>1211</v>
       </c>
       <c r="R223" t="s">
         <v>433</v>
@@ -44005,7 +44003,7 @@
         <v>783</v>
       </c>
       <c r="V223" s="19" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="W223" t="s">
         <v>15</v>
@@ -44120,16 +44118,16 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="C224" t="s">
         <v>374</v>
       </c>
       <c r="D224" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E224" s="2" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="F224" t="s">
         <v>8</v>
@@ -44151,10 +44149,10 @@
         <v>114</v>
       </c>
       <c r="O224" t="s">
+        <v>1260</v>
+      </c>
+      <c r="P224" t="s">
         <v>1261</v>
-      </c>
-      <c r="P224" t="s">
-        <v>1262</v>
       </c>
       <c r="R224" t="s">
         <v>433</v>
@@ -44169,7 +44167,7 @@
         <v>783</v>
       </c>
       <c r="V224" s="19" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="W224" t="s">
         <v>15</v>
@@ -44284,16 +44282,16 @@
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="C225" t="s">
         <v>374</v>
       </c>
       <c r="D225" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E225" s="2" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="F225" t="s">
         <v>8</v>
@@ -44315,10 +44313,10 @@
         <v>443</v>
       </c>
       <c r="O225" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="P225" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="R225" t="s">
         <v>433</v>
@@ -44333,7 +44331,7 @@
         <v>783</v>
       </c>
       <c r="V225" s="19" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="W225" t="s">
         <v>15</v>
@@ -44448,16 +44446,16 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C226" t="s">
         <v>374</v>
       </c>
       <c r="D226" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="E226" s="2" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F226" t="s">
         <v>8</v>
@@ -44479,10 +44477,10 @@
         <v>163</v>
       </c>
       <c r="O226" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="P226" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="R226" t="s">
         <v>433</v>
@@ -44497,7 +44495,7 @@
         <v>783</v>
       </c>
       <c r="V226" s="19" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="W226" t="s">
         <v>15</v>
@@ -44612,16 +44610,16 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="C227" t="s">
         <v>438</v>
       </c>
       <c r="D227" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="E227" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F227" t="s">
         <v>8</v>
@@ -44646,7 +44644,7 @@
         <v>703</v>
       </c>
       <c r="P227" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="R227" t="s">
         <v>433</v>
@@ -44661,7 +44659,7 @@
         <v>783</v>
       </c>
       <c r="V227" s="19" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="W227" t="s">
         <v>15</v>
@@ -44776,16 +44774,16 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="C228" t="s">
         <v>333</v>
       </c>
       <c r="D228" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="E228" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F228" t="s">
         <v>8</v>
@@ -44807,10 +44805,10 @@
         <v>264</v>
       </c>
       <c r="O228" t="s">
+        <v>1273</v>
+      </c>
+      <c r="P228" t="s">
         <v>1274</v>
-      </c>
-      <c r="P228" t="s">
-        <v>1275</v>
       </c>
       <c r="R228" t="s">
         <v>433</v>
@@ -44825,7 +44823,7 @@
         <v>783</v>
       </c>
       <c r="V228" s="19" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="W228" t="s">
         <v>15</v>
@@ -44946,10 +44944,10 @@
         <v>333</v>
       </c>
       <c r="D229" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E229" s="2" t="s">
         <v>1153</v>
-      </c>
-      <c r="E229" s="2" t="s">
-        <v>1154</v>
       </c>
       <c r="F229" t="s">
         <v>8</v>
@@ -45104,7 +45102,7 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C230" t="s">
         <v>113</v>
@@ -45113,7 +45111,7 @@
         <v>145</v>
       </c>
       <c r="E230" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="F230" t="s">
         <v>8</v>
@@ -45135,10 +45133,10 @@
         <v>569</v>
       </c>
       <c r="O230" t="s">
+        <v>1157</v>
+      </c>
+      <c r="P230" t="s">
         <v>1158</v>
-      </c>
-      <c r="P230" t="s">
-        <v>1159</v>
       </c>
       <c r="R230" t="s">
         <v>458</v>
@@ -45153,13 +45151,13 @@
         <v>783</v>
       </c>
       <c r="V230" s="19" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="W230" t="s">
         <v>14</v>
       </c>
       <c r="X230" s="2" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="AA230" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -45271,7 +45269,7 @@
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="C231" t="s">
         <v>113</v>
@@ -45280,10 +45278,10 @@
         <v>114</v>
       </c>
       <c r="E231" s="2" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F231" t="s">
         <v>1167</v>
-      </c>
-      <c r="F231" t="s">
-        <v>1168</v>
       </c>
       <c r="G231" s="3">
         <v>0</v>
@@ -45305,16 +45303,16 @@
         <v>44712</v>
       </c>
       <c r="M231" t="s">
+        <v>1212</v>
+      </c>
+      <c r="N231" s="2" t="s">
         <v>1213</v>
       </c>
-      <c r="N231" s="2" t="s">
-        <v>1214</v>
-      </c>
       <c r="O231" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="P231" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="R231" t="s">
         <v>507</v>
@@ -45326,7 +45324,7 @@
         <v>14</v>
       </c>
       <c r="U231" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="V231" s="19" t="s">
         <v>837</v>
@@ -45335,7 +45333,7 @@
         <v>15</v>
       </c>
       <c r="X231" s="2" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="AA231" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -45447,7 +45445,7 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C232" t="s">
         <v>260</v>
@@ -45456,7 +45454,7 @@
         <v>786</v>
       </c>
       <c r="E232" s="2" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="F232" t="s">
         <v>8</v>
@@ -45478,10 +45476,10 @@
         <v>791</v>
       </c>
       <c r="O232" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="P232" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="R232" t="s">
         <v>433</v>
@@ -45611,7 +45609,7 @@
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="C233" t="s">
         <v>439</v>
@@ -45620,10 +45618,10 @@
         <v>692</v>
       </c>
       <c r="E233" s="2" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="F233" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="G233" s="3">
         <v>0</v>
@@ -45645,16 +45643,16 @@
         <v>44712</v>
       </c>
       <c r="M233" t="s">
+        <v>1215</v>
+      </c>
+      <c r="N233" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="N233" s="2" t="s">
-        <v>1217</v>
-      </c>
       <c r="O233" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="P233" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="R233" t="s">
         <v>507</v>
@@ -45666,7 +45664,7 @@
         <v>14</v>
       </c>
       <c r="U233" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="V233" s="19" t="s">
         <v>864</v>
@@ -45675,7 +45673,7 @@
         <v>15</v>
       </c>
       <c r="X233" s="2" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="AA233" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -45787,7 +45785,7 @@
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="C234" t="s">
         <v>171</v>
@@ -45796,10 +45794,10 @@
         <v>282</v>
       </c>
       <c r="E234" s="2" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="F234" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="G234" s="3">
         <v>0</v>
@@ -45821,16 +45819,16 @@
         <v>44733</v>
       </c>
       <c r="M234" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="N234" s="2" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="O234" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="P234" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="R234" t="s">
         <v>507</v>
@@ -45842,7 +45840,7 @@
         <v>14</v>
       </c>
       <c r="U234" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="V234" s="19" t="s">
         <v>1080</v>
@@ -45851,7 +45849,7 @@
         <v>15</v>
       </c>
       <c r="X234" s="2" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="AA234" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -45963,7 +45961,7 @@
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C235" t="s">
         <v>171</v>
@@ -45972,10 +45970,10 @@
         <v>183</v>
       </c>
       <c r="E235" s="2" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="F235" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="G235" s="3">
         <v>0</v>
@@ -45997,16 +45995,16 @@
         <v>44746</v>
       </c>
       <c r="M235" t="s">
+        <v>1236</v>
+      </c>
+      <c r="N235" s="2" t="s">
+        <v>1235</v>
+      </c>
+      <c r="O235" t="s">
+        <v>1219</v>
+      </c>
+      <c r="P235" t="s">
         <v>1237</v>
-      </c>
-      <c r="N235" s="2" t="s">
-        <v>1236</v>
-      </c>
-      <c r="O235" t="s">
-        <v>1220</v>
-      </c>
-      <c r="P235" t="s">
-        <v>1238</v>
       </c>
       <c r="R235" t="s">
         <v>507</v>
@@ -46018,16 +46016,16 @@
         <v>14</v>
       </c>
       <c r="U235" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="V235" s="19" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="W235" t="s">
         <v>15</v>
       </c>
       <c r="X235" s="2" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="AA235" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -46148,10 +46146,10 @@
         <v>19</v>
       </c>
       <c r="E236" s="2" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="F236" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="G236" s="3">
         <v>0</v>
@@ -46173,16 +46171,16 @@
         <v>44756</v>
       </c>
       <c r="M236" t="s">
+        <v>1241</v>
+      </c>
+      <c r="N236" s="2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="O236" t="s">
+        <v>1170</v>
+      </c>
+      <c r="P236" t="s">
         <v>1242</v>
-      </c>
-      <c r="N236" s="2" t="s">
-        <v>1241</v>
-      </c>
-      <c r="O236" t="s">
-        <v>1171</v>
-      </c>
-      <c r="P236" t="s">
-        <v>1243</v>
       </c>
       <c r="R236" t="s">
         <v>446</v>
@@ -46194,16 +46192,16 @@
         <v>14</v>
       </c>
       <c r="U236" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="V236" s="19" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="W236" t="s">
         <v>15</v>
       </c>
       <c r="X236" s="2" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="AA236" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -46315,7 +46313,7 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="C237" t="s">
         <v>439</v>
@@ -46324,10 +46322,10 @@
         <v>440</v>
       </c>
       <c r="E237" s="2" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="F237" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="G237" s="3">
         <v>0</v>
@@ -46349,16 +46347,16 @@
         <v>44812</v>
       </c>
       <c r="M237" t="s">
+        <v>1248</v>
+      </c>
+      <c r="N237" s="2" t="s">
         <v>1249</v>
       </c>
-      <c r="N237" s="2" t="s">
+      <c r="O237" t="s">
         <v>1250</v>
       </c>
-      <c r="O237" t="s">
+      <c r="P237" t="s">
         <v>1251</v>
-      </c>
-      <c r="P237" t="s">
-        <v>1252</v>
       </c>
       <c r="R237" t="s">
         <v>446</v>
@@ -46370,7 +46368,7 @@
         <v>14</v>
       </c>
       <c r="U237" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="V237" s="19" t="s">
         <v>837</v>
@@ -46379,7 +46377,7 @@
         <v>15</v>
       </c>
       <c r="X237" s="2" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="AA237" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -46491,7 +46489,7 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="C238" t="s">
         <v>260</v>
@@ -46500,7 +46498,7 @@
         <v>317</v>
       </c>
       <c r="E238" s="2" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="F238" t="s">
         <v>8</v>
@@ -46528,10 +46526,10 @@
         <v>147</v>
       </c>
       <c r="O238" t="s">
+        <v>1255</v>
+      </c>
+      <c r="P238" t="s">
         <v>1256</v>
-      </c>
-      <c r="P238" t="s">
-        <v>1257</v>
       </c>
       <c r="R238" t="s">
         <v>446</v>
@@ -46552,7 +46550,7 @@
         <v>15</v>
       </c>
       <c r="X238" s="2" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="AA238" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -46664,7 +46662,7 @@
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="C239" t="s">
         <v>333</v>
@@ -46673,7 +46671,7 @@
         <v>332</v>
       </c>
       <c r="E239" s="2" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="F239" t="s">
         <v>520</v>
@@ -46700,10 +46698,10 @@
         <v>147</v>
       </c>
       <c r="O239" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="P239" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="R239" t="s">
         <v>458</v>
@@ -46833,7 +46831,7 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="C240" t="s">
         <v>333</v>
@@ -46842,7 +46840,7 @@
         <v>332</v>
       </c>
       <c r="E240" s="2" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="F240" t="s">
         <v>149</v>
@@ -46873,7 +46871,7 @@
         <v>150</v>
       </c>
       <c r="P240" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="R240" t="s">
         <v>458</v>
@@ -46888,13 +46886,13 @@
         <v>767</v>
       </c>
       <c r="V240" s="19" t="s">
+        <v>1286</v>
+      </c>
+      <c r="W240" t="s">
+        <v>14</v>
+      </c>
+      <c r="X240" s="2" t="s">
         <v>1287</v>
-      </c>
-      <c r="W240" t="s">
-        <v>14</v>
-      </c>
-      <c r="X240" s="2" t="s">
-        <v>1288</v>
       </c>
       <c r="AA240" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -47006,7 +47004,7 @@
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="C241" t="s">
         <v>333</v>
@@ -47015,7 +47013,7 @@
         <v>332</v>
       </c>
       <c r="E241" s="2" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="F241" t="s">
         <v>149</v>
@@ -47046,7 +47044,7 @@
         <v>150</v>
       </c>
       <c r="P241" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="R241" t="s">
         <v>458</v>
@@ -47061,13 +47059,13 @@
         <v>767</v>
       </c>
       <c r="V241" s="19" t="s">
+        <v>1298</v>
+      </c>
+      <c r="W241" t="s">
+        <v>14</v>
+      </c>
+      <c r="X241" s="2" t="s">
         <v>1299</v>
-      </c>
-      <c r="W241" t="s">
-        <v>14</v>
-      </c>
-      <c r="X241" s="2" t="s">
-        <v>1300</v>
       </c>
       <c r="AA241" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -47179,7 +47177,7 @@
         <v>241</v>
       </c>
       <c r="B242" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="C242" t="s">
         <v>260</v>
@@ -47188,7 +47186,7 @@
         <v>259</v>
       </c>
       <c r="E242" s="2" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="F242" t="s">
         <v>81</v>
@@ -47218,7 +47216,7 @@
         <v>235</v>
       </c>
       <c r="P242" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="R242" t="s">
         <v>458</v>
@@ -47233,13 +47231,13 @@
         <v>785</v>
       </c>
       <c r="V242" s="19" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="W242" t="s">
         <v>15</v>
       </c>
       <c r="X242" s="2" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="AA242" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -47351,16 +47349,16 @@
         <v>242</v>
       </c>
       <c r="B243" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="C243" t="s">
         <v>3</v>
       </c>
       <c r="D243" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="E243" s="2" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="F243" t="s">
         <v>8</v>
@@ -47385,16 +47383,16 @@
         <v>44900</v>
       </c>
       <c r="M243" t="s">
+        <v>1312</v>
+      </c>
+      <c r="N243" s="2" t="s">
         <v>1313</v>
-      </c>
-      <c r="N243" s="2" t="s">
-        <v>1314</v>
       </c>
       <c r="O243" t="s">
         <v>30</v>
       </c>
       <c r="P243" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="R243" t="s">
         <v>507</v>
@@ -47409,13 +47407,13 @@
         <v>783</v>
       </c>
       <c r="V243" s="19" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="W243" t="s">
         <v>15</v>
       </c>
       <c r="X243" s="2" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="AA243" t="str">
         <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
@@ -47893,22 +47891,22 @@
   <sheetData>
     <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
   </sheetData>
@@ -47978,7 +47976,7 @@
         <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -48090,7 +48088,7 @@
         <v>132</v>
       </c>
       <c r="B20" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -48106,7 +48104,7 @@
         <v>137</v>
       </c>
       <c r="B22" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -48234,7 +48232,7 @@
         <v>140</v>
       </c>
       <c r="B38" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -48322,7 +48320,7 @@
         <v>101</v>
       </c>
       <c r="B49" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -48346,7 +48344,7 @@
         <v>134</v>
       </c>
       <c r="B52" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -48506,7 +48504,7 @@
         <v>54</v>
       </c>
       <c r="B72" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -48594,7 +48592,7 @@
         <v>131</v>
       </c>
       <c r="B83" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -48602,7 +48600,7 @@
         <v>126</v>
       </c>
       <c r="B84" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -48626,7 +48624,7 @@
         <v>135</v>
       </c>
       <c r="B87" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -48778,7 +48776,7 @@
         <v>139</v>
       </c>
       <c r="B106" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -48802,7 +48800,7 @@
         <v>141</v>
       </c>
       <c r="B109" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
@@ -48810,7 +48808,7 @@
         <v>127</v>
       </c>
       <c r="B110" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
@@ -48858,7 +48856,7 @@
         <v>130</v>
       </c>
       <c r="B116" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
@@ -48890,7 +48888,7 @@
         <v>125</v>
       </c>
       <c r="B120" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
@@ -49010,7 +49008,7 @@
         <v>128</v>
       </c>
       <c r="B135" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
@@ -49018,7 +49016,7 @@
         <v>129</v>
       </c>
       <c r="B136" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
@@ -49058,7 +49056,7 @@
         <v>133</v>
       </c>
       <c r="B141" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
@@ -49066,7 +49064,7 @@
         <v>138</v>
       </c>
       <c r="B142" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
   </sheetData>
@@ -49397,7 +49395,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -49509,7 +49507,7 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -49677,7 +49675,7 @@
         <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -49701,7 +49699,7 @@
         <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -49789,7 +49787,7 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -49901,7 +49899,7 @@
         <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -49965,7 +49963,7 @@
         <v>76</v>
       </c>
       <c r="B47" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -49981,7 +49979,7 @@
         <v>72</v>
       </c>
       <c r="B49" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -50037,7 +50035,7 @@
         <v>73</v>
       </c>
       <c r="B56" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -50125,7 +50123,7 @@
         <v>71</v>
       </c>
       <c r="B67" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -50141,7 +50139,7 @@
         <v>74</v>
       </c>
       <c r="B69" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -50221,7 +50219,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -50229,7 +50227,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>